<commit_message>
Clean code for eda and calculation
</commit_message>
<xml_diff>
--- a/plots/visualization.xlsx
+++ b/plots/visualization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CHI\2_RESEARCH\Research\DigitalPathology\Code\to-plot\plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8160F1CC-618E-45AA-ACDC-2C75F08BEBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78095BE5-2746-4778-AEB3-FD1C957DD838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{926DE7F2-CDE0-4147-BEE8-7CBD22212D3C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{926DE7F2-CDE0-4147-BEE8-7CBD22212D3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6390,7 +6390,7 @@
   <dimension ref="C3:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>